<commit_message>
setttings and initial_data update
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import.xlsx
+++ b/docs/wordcontrol_import.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="179">
   <si>
     <t>Язык 1</t>
   </si>
@@ -481,13 +481,88 @@
   </si>
   <si>
     <t>поверие</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>viittaa samanmerkityksiseen sanaan, jonka kohdalla on selitys; sulkeissa se on käänöksen edessä</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>viittaa pääartikkeliin, katasanaan tai samakantaiseen sanaan, kantasanasta yhdyssanan, jonka kohdalla, on lisätietoja, tai päinvastoin, synonyymin tai muuhun läheiseen sanaan.</t>
+  </si>
+  <si>
+    <t>ссылка?</t>
+  </si>
+  <si>
+    <t>то же слово, но на каком?</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>merkkiä käytetään rinnakkaismuotojen välillä</t>
+  </si>
+  <si>
+    <t>параллельные?</t>
+  </si>
+  <si>
+    <t>Erottaa eri paikkakuntien ja kylien esimerkit toisistaan. Saman paikkakunnan eri yhteyksissä saadut esimerkit erotta toisistaan piste (vast. kysymys- tai huutomerkki)</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>разные местности и ???</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Esimerkissä osoittaa poistoa.</t>
+  </si>
+  <si>
+    <t>удаление (в примере)</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>В файле две вкладки. Первая — справочная. В соответствии с указанием в ней будут выставлены настройки массовой загрузки.</t>
+  </si>
+  <si>
+    <t>http://slovari.yandex.ru/%D0%BA%D0%BE%D1%88%D0%BA%D0%B0/%D0%BF%D0%B5%D1%80%D0%B5%D0%B2%D0%BE%D0%B4/</t>
+  </si>
+  <si>
+    <t>Вторая — слова и переводы."1" и "2" — это номера языков с первой вкладки.</t>
+  </si>
+  <si>
+    <t>тут ограничением будет "(для лазания на столбы)" или "(электрического крана)".</t>
+  </si>
+  <si>
+    <t>"Написание" — для слова заполняется, если есть официальная орфография. Для ижорского ВСЕГДА пусто.</t>
+  </si>
+  <si>
+    <t>"Произношение" может быть, например, в "учебной", в МФА или просто в той, в которой приведено в источнике. Варианты произношения (или даже написания, такое может быть, если язык имеет несколько литературных норм, как английский) указываются через вертикальную черту. Диалект в скобках (везде одинаково должно быть, например ala и soi).</t>
+  </si>
+  <si>
+    <t>"Часть речи" желательно указывать принятым английским сокращением, но можно и по-русски или по-фински. Главное, чтобы во всём файле было одинаково.</t>
+  </si>
+  <si>
+    <t>"Ограничение перевода" — это, например:</t>
+  </si>
+  <si>
+    <t>vahv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +575,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -565,10 +649,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -586,8 +671,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1071,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,12 +1730,126 @@
       </c>
       <c r="D48" s="4"/>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E48"/>
   <sortState ref="A1:B48">
     <sortCondition ref="A2"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B65" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CSV import works continued
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import.xlsx
+++ b/docs/wordcontrol_import.xlsx
@@ -25,9 +25,6 @@
     <t>Другой язык (основной диалект) [система письма @  источник данных]</t>
   </si>
   <si>
-    <t>синтактическая_категория [классификатор_словоизменения]</t>
-  </si>
-  <si>
     <t>словоформаА1 "комментарий" [грамматическая_категория] [диалект] [информант] | словоформаА2 "комментарий" [грамматическая_категория] [диалект] [информант]</t>
   </si>
   <si>
@@ -41,6 +38,9 @@
   </si>
   <si>
     <t>переводБ1 | переводБ2</t>
+  </si>
+  <si>
+    <t>синтактическая_категория [параметры лексемы] [классификатор_словоизменения]</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,24 +434,24 @@
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extended comment support WIP
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import.xlsx
+++ b/docs/wordcontrol_import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Параметры лексем</t>
   </si>
@@ -28,12 +28,6 @@
     <t>синтактическая_категория</t>
   </si>
   <si>
-    <t>словоформаБ1</t>
-  </si>
-  <si>
-    <t>переводБ1 | переводБ2</t>
-  </si>
-  <si>
     <t xml:space="preserve">словоформаА1 [грамматическая_категория] [диалект] [информант]  "комментарий"  | словоформаА2 [грамматическая_категория] [диалект] [информант] "комментарий" </t>
   </si>
   <si>
@@ -41,6 +35,19 @@
   </si>
   <si>
     <t xml:space="preserve">[тема] [диалект] "комментарий_группы" @  [параметры_лексемы] переводА1 [диалект_перевода] "комментарий_перевода" | [параметры_лексемы] переводА2 [диалект_перевода] "комментарий_перевода" </t>
+  </si>
+  <si>
+    <t>Расширенный комментарий</t>
+  </si>
+  <si>
+    <t>словоформаБ1 *1</t>
+  </si>
+  <si>
+    <t>переводБ1 | переводБ2 *2</t>
+  </si>
+  <si>
+    <t>*1: Расширенный комментарий
+*2: Расширенный комментарий</t>
   </si>
 </sst>
 </file>
@@ -410,18 +417,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="32.5703125" style="2" customWidth="1"/>
+    <col min="1" max="4" width="32.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,27 +438,33 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Literal csv import finished
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import.xlsx
+++ b/docs/wordcontrol_import.xlsx
@@ -19,12 +19,6 @@
     <t>Параметры лексем</t>
   </si>
   <si>
-    <t>Переводимый язык (основной диалект) [система письма @ источник данных]</t>
-  </si>
-  <si>
-    <t>Другой язык (основной диалект) [система письма @  источник данных]</t>
-  </si>
-  <si>
     <t>синтактическая_категория</t>
   </si>
   <si>
@@ -48,6 +42,12 @@
   <si>
     <t>*1: Расширенный комментарий
 *2: Расширенный комментарий</t>
+  </si>
+  <si>
+    <t>Переводимый язык (основной диалект) [система письма] @ источник данных | обработка</t>
+  </si>
+  <si>
+    <t>Другой язык (основной диалект) [система письма] @  источник данных | обработка</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,38 +433,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wordform parsing behaviour changed django_toolbar added
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import.xlsx
+++ b/docs/wordcontrol_import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Параметры лексем</t>
   </si>
@@ -44,10 +44,16 @@
 *2: Расширенный комментарий</t>
   </si>
   <si>
-    <t>Переводимый язык (основной диалект) [система письма] | обработка</t>
-  </si>
-  <si>
-    <t>Другой язык (основной диалект) [система письма] | обработка</t>
+    <t>Переводимый язык (основной диалект) [система письма]</t>
+  </si>
+  <si>
+    <t>словоформаА1 | словоформаА2</t>
+  </si>
+  <si>
+    <t>словоформаБ1</t>
+  </si>
+  <si>
+    <t>Другой язык (основной диалект) [система письма]</t>
   </si>
 </sst>
 </file>
@@ -417,18 +423,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="32.5703125" style="2" customWidth="1"/>
+    <col min="1" max="5" width="32.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,13 +442,16 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -450,10 +459,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -461,9 +473,12 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>